<commit_message>
fix: import plan page, file template
</commit_message>
<xml_diff>
--- a/FinancialPlanningBE/FinancialPlanning.Service/Template/Financial Plan_Template.xlsx
+++ b/FinancialPlanningBE/FinancialPlanning.Service/Template/Financial Plan_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Csharp\FinancialPlanning\financial-planning\FinancialPlanningBE\FinancialPlanning.Service\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FinancialPlanning\FinancialPlanningBE\FinancialPlanning.Service\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AF7954-B8B9-45A3-AFB6-D0B75A4FC8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7637F52-3514-4326-8FCB-3FF4E697BA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28035" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expense plan" sheetId="2" r:id="rId1"/>
@@ -174,7 +174,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;₫&quot;"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;₫&quot;"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -235,7 +235,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,18 +246,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF5E9BD3"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB4C6E7"/>
-        <bgColor rgb="FFB4C6E7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9E1F2"/>
-        <bgColor rgb="FFD9E1F2"/>
       </patternFill>
     </fill>
   </fills>
@@ -274,7 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -282,19 +270,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -310,38 +286,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -626,30 +613,30 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" customWidth="1"/>
-    <col min="10" max="10" width="6.5546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5546875" customWidth="1"/>
-    <col min="12" max="12" width="21.88671875" customWidth="1"/>
-    <col min="13" max="13" width="19.44140625" customWidth="1"/>
-    <col min="14" max="14" width="23.5546875" customWidth="1"/>
-    <col min="15" max="15" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
@@ -662,15 +649,15 @@
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="22"/>
+      <c r="J1" s="12"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
         <v>1</v>
@@ -681,8 +668,8 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:15" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -697,10 +684,10 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="23" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -709,7 +696,7 @@
       <c r="I2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="13" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="2"/>
@@ -726,124 +713,124 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="7"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+    </row>
+    <row r="4" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+    </row>
+    <row r="5" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+    </row>
+    <row r="6" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+    </row>
+    <row r="7" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+    </row>
+    <row r="8" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="21"/>
+    </row>
+    <row r="9" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -887,7 +874,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -901,22 +888,22 @@
       <selection activeCell="E13" sqref="E13:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="1"/>
@@ -941,22 +928,22 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="1"/>
@@ -980,11 +967,11 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>23</v>
@@ -1015,11 +1002,11 @@
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>25</v>
@@ -1050,11 +1037,11 @@
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>27</v>
@@ -1085,11 +1072,11 @@
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>29</v>
@@ -1120,11 +1107,11 @@
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>31</v>
@@ -1153,11 +1140,11 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
-      <c r="AA7" s="5"/>
-      <c r="AB7" s="5"/>
-      <c r="AC7" s="5"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>32</v>
@@ -1186,11 +1173,11 @@
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
-      <c r="AA8" s="5"/>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="5"/>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>33</v>
@@ -1219,11 +1206,11 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
-      <c r="AA9" s="5"/>
-      <c r="AB9" s="5"/>
-      <c r="AC9" s="5"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1250,17 +1237,17 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="5"/>
-      <c r="AC10" s="5"/>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="6" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="1"/>
@@ -1285,22 +1272,22 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
-      <c r="AA11" s="5"/>
-      <c r="AB11" s="5"/>
-      <c r="AC11" s="5"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="1"/>
@@ -1324,11 +1311,11 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
-      <c r="AA12" s="5"/>
-      <c r="AB12" s="5"/>
-      <c r="AC12" s="5"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>36</v>
@@ -1359,11 +1346,11 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
-      <c r="AA13" s="5"/>
-      <c r="AB13" s="5"/>
-      <c r="AC13" s="5"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>38</v>
@@ -1395,7 +1382,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>40</v>
@@ -1427,7 +1414,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>42</v>
@@ -1459,7 +1446,7 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>44</v>
@@ -1491,7 +1478,7 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1519,7 +1506,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1547,7 +1534,7 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>

</xml_diff>